<commit_message>
Update stick diagram mapping
</commit_message>
<xml_diff>
--- a/Documents/01 - Cementing Service Invitation/03 - Request Job Design/Artifacts/Analysis/StickDiagramToEntityMapping.xlsx
+++ b/Documents/01 - Cementing Service Invitation/03 - Request Job Design/Artifacts/Analysis/StickDiagramToEntityMapping.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_metashare\eService_WorkItems\Documents\01 - Cementing Service Invitation\03 - Request Job Design\Artifacts\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C605D6D-6B4F-4199-ADBD-ED154E1D96A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A207E9-477B-4B7D-8D32-64B466652B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{E181215F-33A2-4F43-A4CB-6823152E5153}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{E181215F-33A2-4F43-A4CB-6823152E5153}"/>
   </bookViews>
   <sheets>
     <sheet name="Request Header" sheetId="1" r:id="rId1"/>
-    <sheet name="Open Hole" sheetId="2" r:id="rId2"/>
-    <sheet name="Drill Pipe" sheetId="4" r:id="rId3"/>
-    <sheet name="Tubing" sheetId="5" r:id="rId4"/>
-    <sheet name="CasingPipe" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="RigSetting" sheetId="6" r:id="rId2"/>
+    <sheet name="Formation" sheetId="7" r:id="rId3"/>
+    <sheet name="Open Hole" sheetId="2" r:id="rId4"/>
+    <sheet name="Drill Pipe" sheetId="4" r:id="rId5"/>
+    <sheet name="Tubing" sheetId="5" r:id="rId6"/>
+    <sheet name="CasingPipe" sheetId="3" r:id="rId7"/>
+    <sheet name="BHA" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="144">
   <si>
     <t>Entity Field</t>
   </si>
@@ -113,13 +115,373 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <t>AFENumber</t>
+  </si>
+  <si>
+    <t>AFE#</t>
+  </si>
+  <si>
+    <t>Well.Name</t>
+  </si>
+  <si>
+    <t>Well Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well.SurfaceLocation </t>
+  </si>
+  <si>
+    <t>Surface Location</t>
+  </si>
+  <si>
+    <t>UWI</t>
+  </si>
+  <si>
+    <t>Well.DownholeLocation</t>
+  </si>
+  <si>
+    <t>Bottom Hole Location</t>
+  </si>
+  <si>
+    <t>Well.Licence</t>
+  </si>
+  <si>
+    <t>Licence No</t>
+  </si>
+  <si>
+    <t>GroundLevel</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>KBElevation</t>
+  </si>
+  <si>
+    <t>KB Elevation</t>
+  </si>
+  <si>
+    <t>GLtoKB</t>
+  </si>
+  <si>
+    <t>GL to KB</t>
+  </si>
+  <si>
+    <t>Rig</t>
+  </si>
+  <si>
+    <t>ClientContacts.Title</t>
+  </si>
+  <si>
+    <t>ClientContacts.Name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>STICK DIAGRAM / DRILLING PROGRAM - Montney HZ</t>
+  </si>
+  <si>
+    <t>No Title</t>
+  </si>
+  <si>
+    <t>ClientContacts.Email</t>
+  </si>
+  <si>
+    <t>ClientContacts.Comments</t>
+  </si>
+  <si>
+    <t>ClientContacts.PhoneNumber</t>
+  </si>
+  <si>
+    <t>May not be provided</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Mike Braun</t>
+  </si>
+  <si>
+    <t>(403) 556-9264</t>
+  </si>
+  <si>
+    <t>Supervisors</t>
+  </si>
+  <si>
+    <t>ServiceProviderContacts.Title</t>
+  </si>
+  <si>
+    <t>ServiceProviderContacts.Name</t>
+  </si>
+  <si>
+    <t>ServiceProviderContacts.PhoneNumber</t>
+  </si>
+  <si>
+    <t>ServiceProviderContacts.Email</t>
+  </si>
+  <si>
+    <t>ServiceProviderContacts.Comments</t>
+  </si>
+  <si>
+    <t>Field Operation</t>
+  </si>
+  <si>
+    <t>GP South</t>
+  </si>
+  <si>
+    <t>(780)831-7475</t>
+  </si>
+  <si>
+    <t>OSRContacts.Title</t>
+  </si>
+  <si>
+    <t>OSRContacts.Name</t>
+  </si>
+  <si>
+    <t>OSRContacts.PhoneNumber</t>
+  </si>
+  <si>
+    <t>OSRContacts.Email</t>
+  </si>
+  <si>
+    <t>OSRContacts.Comments</t>
+  </si>
+  <si>
+    <t>Casing Delivery</t>
+  </si>
+  <si>
+    <t>Tenaris Rig Direct</t>
+  </si>
+  <si>
+    <t>(780)766-0310</t>
+  </si>
+  <si>
+    <t>WellLog.LogType</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>MWD Logs</t>
+  </si>
+  <si>
+    <t>WellLog.LoggingCompany</t>
+  </si>
+  <si>
+    <t>Logging Co</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>WellLog.Comments</t>
+  </si>
+  <si>
+    <t>Logging Suite</t>
+  </si>
+  <si>
+    <t>MWD gamma from drill out to TD</t>
+  </si>
+  <si>
+    <t>This section will be specified with each stick diagram</t>
+  </si>
+  <si>
+    <t>FormationType</t>
+  </si>
+  <si>
+    <t>Formation</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Formation</t>
+  </si>
+  <si>
+    <t>Puskwaskau</t>
+  </si>
+  <si>
+    <t>MeausreDepth</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>TrueVerticalDepth</t>
+  </si>
+  <si>
+    <t>TVD</t>
+  </si>
+  <si>
+    <t>MaximumPressure</t>
+  </si>
+  <si>
+    <t>Max Press.</t>
+  </si>
+  <si>
+    <t>MaximumPressureGradient</t>
+  </si>
+  <si>
+    <t>Max GRAD</t>
+  </si>
+  <si>
+    <t>MaximumEstimatedMudDensity</t>
+  </si>
+  <si>
+    <t>ExpectMuDensity</t>
+  </si>
+  <si>
+    <t>Max EMD Per Fmn</t>
+  </si>
+  <si>
+    <t>Expected MWT</t>
+  </si>
+  <si>
+    <t>H2SConcentration</t>
+  </si>
+  <si>
+    <t>H2S</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>IsOverPressureZone</t>
+  </si>
+  <si>
+    <t>IsLossCirculationZone</t>
+  </si>
+  <si>
+    <t>null and 0 has different meaning</t>
+  </si>
+  <si>
+    <t>Need special instruction</t>
+  </si>
+  <si>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>Co 3</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Well.DepthInfo.Label</t>
+  </si>
+  <si>
+    <t>Surface Casing</t>
+  </si>
+  <si>
+    <t>Well.DepthInfo.MeasuredDepth</t>
+  </si>
+  <si>
+    <t>Col 4</t>
+  </si>
+  <si>
+    <t>Well.DepthInfo.TrueVerticalDepth</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Section Title</t>
+  </si>
+  <si>
+    <t>BHA #1: Surface - SCP</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Row 1</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Telemetry</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>NMDC</t>
+  </si>
+  <si>
+    <t>Collars</t>
+  </si>
+  <si>
+    <t>HWDP</t>
+  </si>
+  <si>
+    <t>DPtoSurface</t>
+  </si>
+  <si>
+    <t>DrillingJars</t>
+  </si>
+  <si>
+    <t>311 mm 619 PDC</t>
+  </si>
+  <si>
+    <t>Slick MM – 9 7/8", 7.0 stg, 1.83° Adj, 0.047 rev/L</t>
+  </si>
+  <si>
+    <t>PHX Velocity</t>
+  </si>
+  <si>
+    <t>X/O Sub, Gap Sub</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>8 × 6.25" DCs</t>
+  </si>
+  <si>
+    <t>Row 5</t>
+  </si>
+  <si>
+    <t>Row 7</t>
+  </si>
+  <si>
+    <t>Row 9</t>
+  </si>
+  <si>
+    <t>Maybe match Sub</t>
+  </si>
+  <si>
+    <t>Row 2,3</t>
+  </si>
+  <si>
+    <t>Row 4, 6</t>
+  </si>
+  <si>
+    <t>Row 10</t>
+  </si>
+  <si>
+    <t>Row 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114.3 mm </t>
+  </si>
+  <si>
+    <t>split 2</t>
+  </si>
+  <si>
+    <t>Split 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +501,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,10 +532,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,21 +872,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1DC009-4818-4351-A966-9472F242D4E5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,10 +900,461 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7628AB-C749-4797-BCC1-2D7ED29BAC9B}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +1362,192 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F421686-0BA4-4321-8E48-E747D9B5E95B}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6">
+        <v>9234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BE37E1-D6D2-4385-B5B9-FBF0BBBB4E9B}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -604,7 +1613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EAD631-01B9-4257-8B04-94EFA1063B0D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -653,7 +1662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9766333B-B7DC-45D1-B0EE-6DFB9D34A7A7}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -698,13 +1707,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CD0EEA-AD9C-41FD-A8E7-DE73C9303A8C}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -838,17 +1845,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7628AB-C749-4797-BCC1-2D7ED29BAC9B}">
-  <dimension ref="A1:F1"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10644717-BC17-4837-8949-31AA54571320}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,19 +1872,145 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>